<commit_message>
included limitation of feed-in and EEG-levy on on-site consumed generated power
</commit_message>
<xml_diff>
--- a/Linearisierungen/HP Kosten.xlsx
+++ b/Linearisierungen/HP Kosten.xlsx
@@ -1,60 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_16144C204AC08FBF8F99CDAFECFBC4FD58A2A27E" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{F5796CF5-0DF3-4A93-8C63-57385D1DE7D5}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_16144C204AC08FBF8F99CDAFECFBC4FD58A2A27E" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{5FA7B75E-9092-4B0B-98CE-FBC76E166B56}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4185" yWindow="4185" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4185" yWindow="4185" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Diagramm1" sheetId="2" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Tabelle1!$I$3:$I$5</definedName>
-    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Tabelle1!$F$9</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Tabelle1!$F$8</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Tabelle1!$F$7</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Tabelle1!$F$7</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Tabelle1!$F$7</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Tabelle1!$F$8</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Tabelle1!$F$9</definedName>
-    <definedName name="solver_lhs8" localSheetId="0" hidden="1">Tabelle1!$F$14</definedName>
-    <definedName name="solver_lhs9" localSheetId="0" hidden="1">Tabelle1!$F$14</definedName>
-    <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Tabelle1!$I$6</definedName>
-    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel7" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs7" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs8" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs9" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_tim" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_tol" localSheetId="0" hidden="1">0.05</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Tabelle1!$I$3:$I$5</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Tabelle1!$F$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Tabelle1!$F$8</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Tabelle1!$F$7</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Tabelle1!$F$7</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Tabelle1!$F$7</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">Tabelle1!$F$8</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">Tabelle1!$F$9</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">Tabelle1!$F$14</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">Tabelle1!$F$14</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Tabelle1!$I$6</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel7" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel9" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs9" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.05</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -205,7 +206,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Bundesministerium</c:v>
+            <c:v>BMVBS Publikation</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -292,7 +293,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1690-4E0C-9321-A7431AD09CDF}"/>
+              <c16:uniqueId val="{00000000-8063-4DAB-9838-05EBFC0B60B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -300,7 +301,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>IER</c:v>
+            <c:v>IER Forschungsbericht</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -417,7 +418,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1690-4E0C-9321-A7431AD09CDF}"/>
+              <c16:uniqueId val="{00000001-8063-4DAB-9838-05EBFC0B60B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -425,7 +426,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>TGA</c:v>
+            <c:v>TGA Bericht</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -488,7 +489,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1690-4E0C-9321-A7431AD09CDF}"/>
+              <c16:uniqueId val="{00000002-8063-4DAB-9838-05EBFC0B60B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -509,10 +510,11 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:trendline>
+            <c:name>Regression</c:name>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:srgbClr val="C00000"/>
                 </a:solidFill>
                 <a:prstDash val="solid"/>
               </a:ln>
@@ -522,37 +524,7 @@
             <c:backward val="6.6"/>
             <c:intercept val="0"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -707,7 +679,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-1690-4E0C-9321-A7431AD09CDF}"/>
+              <c16:uniqueId val="{00000004-8063-4DAB-9838-05EBFC0B60B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -715,7 +687,7 @@
           <c:idx val="5"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>TGA</c:v>
+            <c:v>TGA Bericht</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -790,7 +762,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-1690-4E0C-9321-A7431AD09CDF}"/>
+              <c16:uniqueId val="{00000005-8063-4DAB-9838-05EBFC0B60B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -810,15 +782,16 @@
           </c:marker>
           <c:trendline>
             <c:spPr>
-              <a:ln w="19050"/>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:intercept val="120"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -907,7 +880,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0D06-49A6-A5E9-8F70452C3D46}"/>
+              <c16:uniqueId val="{00000007-8063-4DAB-9838-05EBFC0B60B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -997,7 +970,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E013-4181-B5A1-D548EB9E4084}"/>
+              <c16:uniqueId val="{00000008-8063-4DAB-9838-05EBFC0B60B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1016,6 +989,7 @@
         <c:axId val="81874944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="4000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1023,9 +997,8 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1033,18 +1006,49 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1500"/>
+                  <a:t>Nennwärmeleistung</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1500" baseline="0"/>
+                  <a:t> [MW] </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1500"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1055,12 +1059,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1073,6 +1074,9 @@
         <c:crossAx val="81876480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
       </c:valAx>
       <c:valAx>
         <c:axId val="81876480"/>
@@ -1085,9 +1089,8 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1095,18 +1098,44 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1500"/>
+                  <a:t>Investitionskosten [Tsd. €]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1117,12 +1146,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1135,15 +1161,76 @@
         <c:crossAx val="81874944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:minorUnit val="25"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
-          <a:noFill/>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="6"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="8"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14655471065795278"/>
+          <c:y val="0.10831908212869823"/>
+          <c:w val="0.2236463051754663"/>
+          <c:h val="0.19370502427127528"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1160,12 +1247,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1180,39 +1262,38 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{7F607190-9C63-4AA7-B72D-880359E5D91D}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>11206</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>15967</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>502024</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>1680</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9301370" cy="5996609"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25EFBA81-9AC3-4E32-975A-B0A9AE3111B8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85CA023E-D39A-4763-BFE7-48C0026F464E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1225,7 +1306,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1494,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T28" sqref="T28"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,6 +2009,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>